<commit_message>
update metadata and table
</commit_message>
<xml_diff>
--- a/Tables/Stream_Habitat_ExchangeSpecifications.xlsx
+++ b/Tables/Stream_Habitat_ExchangeSpecifications.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="432">
   <si>
     <t xml:space="preserve">TermID</t>
   </si>
@@ -403,9 +403,84 @@
     <t xml:space="preserve">LongName</t>
   </si>
   <si>
+    <t xml:space="preserve">Channel Characteristics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaver Sign at Reach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beaver value from the provider dataset.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PctDry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of Reach that is Dry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of the reach that was dry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min: 0, max: 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sinuosity of Local Stream Reach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reach sinuosity (reach length along the thalweg divided by straight line distance between the bottom of the reach and the top of the reach)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StreamOrder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stream Order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strahler stream order of the site from the provider dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Channel dimensions</t>
   </si>
   <si>
+    <t xml:space="preserve">AvgBFWDRatio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bankfull width to depth ratio at transects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average bankfull width/depth ratio for the reach.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFHeight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bankfull Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average bankfull height measured from water surface across transects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
     <t xml:space="preserve">BFWidth</t>
   </si>
   <si>
@@ -415,22 +490,16 @@
     <t xml:space="preserve">Average bankfull width across transects for the reach.</t>
   </si>
   <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Channel Characteristics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sinuosity of Local Stream Reach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reach sinuosity (reach length along the thalweg divided by straight line distance between the bottom of the reach and the top of the reach)</t>
+    <t xml:space="preserve">countTransectsBFWidth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count of cross sections</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of cross sections included in the average bankfull width calculation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">count of measurments</t>
   </si>
   <si>
     <t xml:space="preserve">Grad</t>
@@ -442,22 +511,13 @@
     <t xml:space="preserve">Mean slope of water surface (%) from the bottom of the reach to the top of the reach.</t>
   </si>
   <si>
-    <t xml:space="preserve">min: 0, max: 100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PctDry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent of Reach that is Dry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent of the reach that was dry</t>
+    <t xml:space="preserve">MeanThalwegDepth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Thalweg Depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean thalweg depth. Metric of how deep water was at the site.</t>
   </si>
   <si>
     <t xml:space="preserve">ReachLen</t>
@@ -472,48 +532,27 @@
     <t xml:space="preserve">4000</t>
   </si>
   <si>
-    <t xml:space="preserve">Beaver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beaver Sign at Reach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beaver value from the provider dataset.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AvgBFWDRatio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bankfull width to depth ratio at transects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average bankfull width/depth ratio for the reach.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StreamOrder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stream Order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Strahler stream order of the site from the provider dataset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BFHeight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bankfull Height</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average bankfull height measured from water surface across transects.</t>
+    <t xml:space="preserve">WetWidth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average wetted width from transects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average wetted width across transects.</t>
   </si>
   <si>
     <t xml:space="preserve">Pools</t>
   </si>
   <si>
+    <t xml:space="preserve">PctPool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent pools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of the sample reach (linear extent) classified as pool habitat</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPD</t>
   </si>
   <si>
@@ -523,24 +562,6 @@
     <t xml:space="preserve">Average of the residual pool depth values for all pools in a reach. Residual pool depth the difference of the pool tail depth from the max depth.</t>
   </si>
   <si>
-    <t xml:space="preserve">WetWidth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average wetted width from transects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average wetted width across transects.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PctPool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent pools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent of the sample reach (linear extent) classified as pool habitat</t>
-  </si>
-  <si>
     <t xml:space="preserve">Streambanks</t>
   </si>
   <si>
@@ -574,6 +595,24 @@
     <t xml:space="preserve">Substrate</t>
   </si>
   <si>
+    <t xml:space="preserve">D16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diameter of the 16th percentile streambed particle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bed surface particle size corresponding to the 16th percentile of measured particles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min: 1, max: 4098</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4098</t>
+  </si>
+  <si>
     <t xml:space="preserve">D50</t>
   </si>
   <si>
@@ -583,13 +622,22 @@
     <t xml:space="preserve">Median diameter of bed surface particle size corresponding to the areal median (50th percentile of measured particles) .</t>
   </si>
   <si>
-    <t xml:space="preserve">min: 1, max: 4098</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4098</t>
+    <t xml:space="preserve">D84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diameter of the 84th percentile streambed particle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bed surface particle size corresponding to the 84th percentile of measured particles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PctBdrk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent Bed Surface Bedrock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent of the stream bed area that is composed of particles with a b-axis &gt; 4098mm (bedrock)</t>
   </si>
   <si>
     <t xml:space="preserve">PctFines2</t>
@@ -610,33 +658,6 @@
     <t xml:space="preserve">Percent of the stream bed area that is composed of particles with a b-axis &lt; 6 mm</t>
   </si>
   <si>
-    <t xml:space="preserve">D16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diameter of the 16th percentile streambed particle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bed surface particle size corresponding to the 16th percentile of measured particles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diameter of the 84th percentile streambed particle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bed surface particle size corresponding to the 84th percentile of measured particles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PctBdrk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent Bed Surface Bedrock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent of the stream bed area that is composed of particles with a b-axis &gt; 4098mm (bedrock)</t>
-  </si>
-  <si>
     <t xml:space="preserve">PoolTailFines2</t>
   </si>
   <si>
@@ -655,21 +676,6 @@
     <t xml:space="preserve">Average percent fine sediment (&lt; 6mm) on the pool tail</t>
   </si>
   <si>
-    <t xml:space="preserve">MeanThalwegDepth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average Thalweg Depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mean thalweg depth. Metric of how deep water was at the site.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Count of Transects</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of transects in the reach.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Water chemistry</t>
   </si>
   <si>
@@ -682,6 +688,36 @@
     <t xml:space="preserve">ppm</t>
   </si>
   <si>
+    <t xml:space="preserve">pH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measured pH value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min: 0, max: 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SpecificConductance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specific Conductance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Measured specific conductance value. The specific conductance is conductivity standardized to 25 degrees C.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min: 0, max: 65500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uS/cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65500</t>
+  </si>
+  <si>
     <t xml:space="preserve">TotalNitrogen</t>
   </si>
   <si>
@@ -703,36 +739,6 @@
     <t xml:space="preserve">Measured total phosphorous value</t>
   </si>
   <si>
-    <t xml:space="preserve">SpecificConductance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specific Conductance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured specific conductance value. The specific conductance is conductivity standardized to 25 degrees C.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min: 0, max: 65500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uS/cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Measured pH value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">min: 0, max: 14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
     <t xml:space="preserve">Turbidity</t>
   </si>
   <si>
@@ -742,18 +748,6 @@
     <t xml:space="preserve">NTU</t>
   </si>
   <si>
-    <t xml:space="preserve">countTransectsBFWidth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Count of cross sections</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number of cross sections included in the average bankfull width calculation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">count of measurments</t>
-  </si>
-  <si>
     <t xml:space="preserve">AREMPField</t>
   </si>
   <si>
@@ -937,12 +931,126 @@
     <t xml:space="preserve">Yr</t>
   </si>
   <si>
+    <t xml:space="preserve">beaver_impacted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BVR_SGN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCT_DRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/CustomizedMethod/Details/31137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCT_DRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/1610</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StrmFlow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tbd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SNSTY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/3807</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRM_ORDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STRAHLERORDER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ave_widthDepth_ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6849 AND https://www.monitoringresources.org/Document/CustomizedMethod/Details/31107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/1064 OR www.monitoringresources.org/Document/Method/Details/1275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BFWD_RAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6870 AND www.monitoringresources.org/Document/Method/Details/56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/1064 OR  www.monitoringresources.org/Document/Method/Details/1275</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WDTrans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/65 AND https://www.monitoringresources.org/Document/Method/Details/6871</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average_bfdepth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/CustomizedMethod/Details/31107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BNKFLL_HT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BankfullHeightAvg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XBKF_H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7014</t>
+  </si>
+  <si>
     <t xml:space="preserve">average_bfwidth</t>
   </si>
   <si>
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6849</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/4103</t>
+  </si>
+  <si>
     <t xml:space="preserve">BNKFLL_WT</t>
   </si>
   <si>
@@ -964,12 +1072,6 @@
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6871</t>
   </si>
   <si>
-    <t xml:space="preserve">SNSTY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SINU</t>
-  </si>
-  <si>
     <t xml:space="preserve">gradient</t>
   </si>
   <si>
@@ -982,82 +1084,97 @@
     <t xml:space="preserve">PctSlope</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.monitoringresources.org/Document/CustomizedMethod/Details/31139</t>
+    <t xml:space="preserve">www.monitoringresources.org/Document/CustomizedMethod/Details/31139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/4113</t>
   </si>
   <si>
     <t xml:space="preserve">XSLOPE</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6868</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCT_DRY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PctDru</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCT_DRS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrmFlow</t>
+    <t xml:space="preserve">ThalwegDepthMean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XDEPTH_CM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7015</t>
   </si>
   <si>
     <t xml:space="preserve">REACH_LENGTH</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/3807</t>
-  </si>
-  <si>
     <t xml:space="preserve">TOT_RCH_LEN</t>
   </si>
   <si>
     <t xml:space="preserve">ProtocolReachLength</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7017</t>
+  </si>
+  <si>
     <t xml:space="preserve">REACHLEN</t>
   </si>
   <si>
     <t xml:space="preserve">RchLen</t>
   </si>
   <si>
-    <t xml:space="preserve">beaver_impacted</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BVR_SGN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ave_widthDepth_ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BFWD_RAT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WDTrans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRM_ORDR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STRAHLERORDER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">average_bfdepth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BNKFLL_HT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BankfullHeightAvg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XBKF_H</t>
+    <t xml:space="preserve">wettedWidth_ave</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/3893</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WTTD_WT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WettedWidthAvg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XWIDTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PctReachInPools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6844</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/3852</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCT_PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PctPools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6859</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/4115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PoolPct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6872</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/55</t>
   </si>
   <si>
     <t xml:space="preserve">ave_residual_depth</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6844</t>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6976</t>
   </si>
   <si>
     <t xml:space="preserve">RES_PL_DEP</t>
@@ -1066,48 +1183,9 @@
     <t xml:space="preserve">ResPoolDepthAvg</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6859</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6875</t>
-  </si>
-  <si>
     <t xml:space="preserve">PoolDp</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6872</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wettedWidth_ave</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WTTD_WT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WettedWidthAvg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XWIDTH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PctReachInPools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/3852</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCT_PL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PctPools</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PoolPct</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/55</t>
-  </si>
-  <si>
     <t xml:space="preserve">BNK_AN</t>
   </si>
   <si>
@@ -1117,15 +1195,24 @@
     <t xml:space="preserve">BNK_STBLTY</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7010</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stab</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/69</t>
-  </si>
-  <si>
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6797</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6810</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/1730</t>
+  </si>
+  <si>
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6801</t>
   </si>
   <si>
@@ -1135,9 +1222,21 @@
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6874</t>
   </si>
   <si>
+    <t xml:space="preserve">bedrock_pcnt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCT_BDRK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7011</t>
+  </si>
+  <si>
     <t xml:space="preserve">pcnt_fines_tran2</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6977</t>
+  </si>
+  <si>
     <t xml:space="preserve">PCT_FN</t>
   </si>
   <si>
@@ -1159,21 +1258,15 @@
     <t xml:space="preserve">PctFinesLessThan6mm</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6810</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bedrock_pcnt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCT_BDRK</t>
-  </si>
-  <si>
     <t xml:space="preserve">pool_fines</t>
   </si>
   <si>
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6798</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/868</t>
+  </si>
+  <si>
     <t xml:space="preserve">PL_TL_FN</t>
   </si>
   <si>
@@ -1186,43 +1279,46 @@
     <t xml:space="preserve">PTFines6</t>
   </si>
   <si>
-    <t xml:space="preserve">ThalwegDepthMean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XDEPTH_CM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/5537</t>
-  </si>
-  <si>
     <t xml:space="preserve">TSS</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/3792</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cond</t>
   </si>
   <si>
     <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/61</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/6673</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/72</t>
+  </si>
+  <si>
     <t xml:space="preserve">NTL</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/548</t>
+  </si>
+  <si>
     <t xml:space="preserve">PTL</t>
   </si>
   <si>
-    <t xml:space="preserve">COND</t>
-  </si>
-  <si>
     <t xml:space="preserve">TRBDTY</t>
   </si>
   <si>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7012</t>
+  </si>
+  <si>
     <t xml:space="preserve">TURB</t>
   </si>
   <si>
-    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/3806</t>
+    <t xml:space="preserve">www.monitoringresources.org/Document/Method/Details/7016</t>
   </si>
 </sst>
 </file>
@@ -2890,7 +2986,7 @@
         <v>126</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>127</v>
@@ -2905,11 +3001,9 @@
       <c r="I2" t="s">
         <v>64</v>
       </c>
-      <c r="J2" t="s">
-        <v>130</v>
-      </c>
+      <c r="J2"/>
       <c r="K2" t="s">
-        <v>131</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
@@ -2920,27 +3014,31 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" t="n">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G3" t="s">
         <v>132</v>
       </c>
-      <c r="D3" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="H3" t="s">
         <v>133</v>
       </c>
-      <c r="F3" t="s">
-        <v>134</v>
-      </c>
-      <c r="G3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H3"/>
       <c r="I3" t="s">
         <v>64</v>
       </c>
-      <c r="J3"/>
+      <c r="J3" t="s">
+        <v>134</v>
+      </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4">
@@ -2954,7 +3052,7 @@
         <v>126</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
         <v>136</v>
@@ -2965,17 +3063,13 @@
       <c r="G4" t="s">
         <v>138</v>
       </c>
-      <c r="H4" t="s">
-        <v>139</v>
-      </c>
+      <c r="H4"/>
       <c r="I4" t="s">
         <v>64</v>
       </c>
-      <c r="J4" t="s">
-        <v>140</v>
-      </c>
+      <c r="J4"/>
       <c r="K4" t="s">
-        <v>141</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
@@ -2986,31 +3080,29 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D5" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="G5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H5" t="s">
-        <v>139</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="H5"/>
       <c r="I5" t="s">
         <v>64</v>
       </c>
       <c r="J5" t="s">
-        <v>140</v>
+        <v>19</v>
       </c>
       <c r="K5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6">
@@ -3021,29 +3113,29 @@
         <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="D6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
+        <v>144</v>
+      </c>
+      <c r="F6" t="s">
         <v>145</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>146</v>
-      </c>
-      <c r="G6" t="s">
-        <v>147</v>
       </c>
       <c r="H6"/>
       <c r="I6" t="s">
         <v>64</v>
       </c>
       <c r="J6" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="K6" t="s">
-        <v>148</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7">
@@ -3054,27 +3146,29 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D7" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F7" t="s">
         <v>149</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>150</v>
-      </c>
-      <c r="G7" t="s">
-        <v>151</v>
       </c>
       <c r="H7"/>
       <c r="I7" t="s">
         <v>64</v>
       </c>
-      <c r="J7"/>
+      <c r="J7" t="s">
+        <v>147</v>
+      </c>
       <c r="K7" t="s">
-        <v>19</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8">
@@ -3085,10 +3179,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
         <v>152</v>
@@ -3104,10 +3198,10 @@
         <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="K8" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9">
@@ -3118,10 +3212,10 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="D9" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
         <v>155</v>
@@ -3137,10 +3231,10 @@
         <v>64</v>
       </c>
       <c r="J9" t="s">
-        <v>19</v>
+        <v>158</v>
       </c>
       <c r="K9" t="s">
-        <v>158</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10">
@@ -3151,10 +3245,10 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="D10" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
         <v>159</v>
@@ -3165,15 +3259,17 @@
       <c r="G10" t="s">
         <v>161</v>
       </c>
-      <c r="H10"/>
+      <c r="H10" t="s">
+        <v>133</v>
+      </c>
       <c r="I10" t="s">
         <v>64</v>
       </c>
       <c r="J10" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="K10" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11">
@@ -3184,29 +3280,29 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" t="n">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
         <v>162</v>
       </c>
-      <c r="D11" t="n">
-        <v>14</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>163</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>164</v>
-      </c>
-      <c r="G11" t="s">
-        <v>165</v>
       </c>
       <c r="H11"/>
       <c r="I11" t="s">
         <v>64</v>
       </c>
       <c r="J11" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="K11" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12">
@@ -3217,29 +3313,29 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="D12" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E12" t="s">
+        <v>165</v>
+      </c>
+      <c r="F12" t="s">
         <v>166</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>167</v>
-      </c>
-      <c r="G12" t="s">
-        <v>168</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="s">
         <v>64</v>
       </c>
       <c r="J12" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="K12" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13">
@@ -3250,10 +3346,10 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="D13" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
         <v>169</v>
@@ -3264,17 +3360,15 @@
       <c r="G13" t="s">
         <v>171</v>
       </c>
-      <c r="H13" t="s">
-        <v>139</v>
-      </c>
+      <c r="H13"/>
       <c r="I13" t="s">
         <v>64</v>
       </c>
       <c r="J13" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="K13" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="14">
@@ -3288,7 +3382,7 @@
         <v>172</v>
       </c>
       <c r="D14" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14" t="s">
         <v>173</v>
@@ -3300,16 +3394,16 @@
         <v>175</v>
       </c>
       <c r="H14" t="s">
-        <v>176</v>
+        <v>133</v>
       </c>
       <c r="I14" t="s">
         <v>64</v>
       </c>
       <c r="J14" t="s">
-        <v>177</v>
+        <v>134</v>
       </c>
       <c r="K14" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15">
@@ -3323,28 +3417,26 @@
         <v>172</v>
       </c>
       <c r="D15" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F15" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="G15" t="s">
-        <v>181</v>
-      </c>
-      <c r="H15" t="s">
-        <v>139</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="H15"/>
       <c r="I15" t="s">
         <v>64</v>
       </c>
       <c r="J15" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="K15" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16">
@@ -3355,31 +3447,31 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
+        <v>179</v>
+      </c>
+      <c r="D16" t="n">
+        <v>16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16" t="s">
+        <v>181</v>
+      </c>
+      <c r="G16" t="s">
         <v>182</v>
       </c>
-      <c r="D16" t="n">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="H16" t="s">
         <v>183</v>
-      </c>
-      <c r="F16" t="s">
-        <v>184</v>
-      </c>
-      <c r="G16" t="s">
-        <v>185</v>
-      </c>
-      <c r="H16" t="s">
-        <v>186</v>
       </c>
       <c r="I16" t="s">
         <v>64</v>
       </c>
       <c r="J16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="K16" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17">
@@ -3390,31 +3482,31 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D17" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E17" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="G17" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="H17" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="I17" t="s">
         <v>64</v>
       </c>
       <c r="J17" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="K17" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18">
@@ -3425,31 +3517,31 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D18" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E18" t="s">
+        <v>190</v>
+      </c>
+      <c r="F18" t="s">
+        <v>191</v>
+      </c>
+      <c r="G18" t="s">
         <v>192</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>193</v>
-      </c>
-      <c r="G18" t="s">
-        <v>194</v>
-      </c>
-      <c r="H18" t="s">
-        <v>139</v>
       </c>
       <c r="I18" t="s">
         <v>64</v>
       </c>
       <c r="J18" t="s">
-        <v>140</v>
+        <v>194</v>
       </c>
       <c r="K18" t="s">
-        <v>141</v>
+        <v>195</v>
       </c>
     </row>
     <row r="19">
@@ -3460,31 +3552,31 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D19" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F19" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H19" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I19" t="s">
         <v>64</v>
       </c>
       <c r="J19" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="K19" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="20">
@@ -3495,31 +3587,31 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D20" t="n">
         <v>22</v>
       </c>
       <c r="E20" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F20" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G20" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H20" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I20" t="s">
         <v>64</v>
       </c>
       <c r="J20" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="K20" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
     </row>
     <row r="21">
@@ -3530,28 +3622,28 @@
         <v>7</v>
       </c>
       <c r="C21" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D21" t="n">
         <v>23</v>
       </c>
       <c r="E21" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F21" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="G21" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H21" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="I21" t="s">
         <v>64</v>
       </c>
       <c r="J21" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="K21" t="s">
         <v>119</v>
@@ -3565,31 +3657,31 @@
         <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D22" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F22" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G22" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="H22" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="I22" t="s">
         <v>64</v>
       </c>
       <c r="J22" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="K22" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23">
@@ -3600,31 +3692,31 @@
         <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D23" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F23" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G23" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H23" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="I23" t="s">
         <v>64</v>
       </c>
       <c r="J23" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="K23" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24">
@@ -3635,29 +3727,31 @@
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="D24" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F24" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G24" t="s">
-        <v>212</v>
-      </c>
-      <c r="H24"/>
+        <v>213</v>
+      </c>
+      <c r="H24" t="s">
+        <v>133</v>
+      </c>
       <c r="I24" t="s">
         <v>64</v>
       </c>
       <c r="J24" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="K24" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25">
@@ -3668,23 +3762,31 @@
         <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="D25" t="n">
-        <v>9</v>
-      </c>
-      <c r="E25"/>
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>214</v>
+      </c>
       <c r="F25" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="G25" t="s">
-        <v>214</v>
-      </c>
-      <c r="H25"/>
-      <c r="I25"/>
-      <c r="J25"/>
+        <v>216</v>
+      </c>
+      <c r="H25" t="s">
+        <v>133</v>
+      </c>
+      <c r="I25" t="s">
+        <v>64</v>
+      </c>
+      <c r="J25" t="s">
+        <v>134</v>
+      </c>
       <c r="K25" t="s">
-        <v>119</v>
+        <v>135</v>
       </c>
     </row>
     <row r="26">
@@ -3695,26 +3797,26 @@
         <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D26" t="n">
         <v>60</v>
       </c>
       <c r="E26" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F26" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="G26" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H26"/>
       <c r="I26" t="s">
         <v>64</v>
       </c>
       <c r="J26" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="K26" t="s">
         <v>119</v>
@@ -3728,29 +3830,31 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D27" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="F27" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="G27" t="s">
-        <v>221</v>
-      </c>
-      <c r="H27"/>
+        <v>222</v>
+      </c>
+      <c r="H27" t="s">
+        <v>223</v>
+      </c>
       <c r="I27" t="s">
         <v>64</v>
       </c>
       <c r="J27" t="s">
-        <v>222</v>
+        <v>19</v>
       </c>
       <c r="K27" t="s">
-        <v>131</v>
+        <v>224</v>
       </c>
     </row>
     <row r="28">
@@ -3761,29 +3865,31 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D28" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="F28" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="G28" t="s">
-        <v>225</v>
-      </c>
-      <c r="H28"/>
+        <v>227</v>
+      </c>
+      <c r="H28" t="s">
+        <v>228</v>
+      </c>
       <c r="I28" t="s">
         <v>64</v>
       </c>
       <c r="J28" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="K28" t="s">
-        <v>131</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29">
@@ -3794,31 +3900,29 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D29" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E29" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="F29" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="G29" t="s">
-        <v>228</v>
-      </c>
-      <c r="H29" t="s">
-        <v>229</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="H29"/>
       <c r="I29" t="s">
         <v>64</v>
       </c>
       <c r="J29" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="K29" t="s">
-        <v>231</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30">
@@ -3829,31 +3933,29 @@
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D30" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F30" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="G30" t="s">
-        <v>233</v>
-      </c>
-      <c r="H30" t="s">
-        <v>234</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="H30"/>
       <c r="I30" t="s">
         <v>64</v>
       </c>
       <c r="J30" t="s">
-        <v>19</v>
+        <v>234</v>
       </c>
       <c r="K30" t="s">
-        <v>235</v>
+        <v>151</v>
       </c>
     </row>
     <row r="31">
@@ -3864,62 +3966,29 @@
         <v>7</v>
       </c>
       <c r="C31" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D31" t="n">
         <v>65</v>
       </c>
       <c r="E31" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F31" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="G31" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H31"/>
       <c r="I31" t="s">
         <v>64</v>
       </c>
       <c r="J31" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="K31" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="n">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>126</v>
-      </c>
-      <c r="D32" t="n">
-        <v>2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>239</v>
-      </c>
-      <c r="F32" t="s">
-        <v>240</v>
-      </c>
-      <c r="G32" t="s">
-        <v>241</v>
-      </c>
-      <c r="H32"/>
-      <c r="I32" t="s">
-        <v>64</v>
-      </c>
-      <c r="J32" t="s">
-        <v>242</v>
-      </c>
-      <c r="K32" t="s">
-        <v>119</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -3965,43 +4034,43 @@
         <v>120</v>
       </c>
       <c r="J1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K1" t="s">
+        <v>242</v>
+      </c>
+      <c r="L1" t="s">
         <v>243</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>244</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>245</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>246</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>247</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>248</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>249</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>250</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>251</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>252</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>253</v>
-      </c>
-      <c r="U1" t="s">
-        <v>254</v>
-      </c>
-      <c r="V1" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="2">
@@ -4084,7 +4153,7 @@
         <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F4" t="s">
         <v>29</v>
@@ -4120,7 +4189,7 @@
         <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F5" t="s">
         <v>34</v>
@@ -4188,7 +4257,7 @@
         <v>38</v>
       </c>
       <c r="E7" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F7" t="s">
         <v>39</v>
@@ -4224,7 +4293,7 @@
         <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F8" t="s">
         <v>43</v>
@@ -4294,7 +4363,7 @@
         <v>48</v>
       </c>
       <c r="E10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F10" t="s">
         <v>49</v>
@@ -4328,7 +4397,7 @@
         <v>50</v>
       </c>
       <c r="E11" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
@@ -4364,7 +4433,7 @@
         <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="F12" t="s">
         <v>57</v>
@@ -4377,25 +4446,25 @@
       </c>
       <c r="I12"/>
       <c r="J12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="K12"/>
       <c r="L12"/>
       <c r="M12" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="N12" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="O12"/>
       <c r="P12"/>
       <c r="Q12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="R12"/>
       <c r="S12"/>
       <c r="T12" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="U12"/>
       <c r="V12"/>
@@ -4410,7 +4479,7 @@
         <v>59</v>
       </c>
       <c r="E13" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F13" t="s">
         <v>60</v>
@@ -4424,10 +4493,10 @@
       <c r="K13"/>
       <c r="L13"/>
       <c r="M13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="N13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="O13"/>
       <c r="P13"/>
@@ -4435,7 +4504,7 @@
       <c r="R13"/>
       <c r="S13"/>
       <c r="T13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="U13"/>
       <c r="V13"/>
@@ -4450,7 +4519,7 @@
         <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="F14" t="s">
         <v>63</v>
@@ -4461,25 +4530,25 @@
       </c>
       <c r="I14"/>
       <c r="J14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K14"/>
       <c r="L14"/>
       <c r="M14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="N14" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="R14"/>
       <c r="S14"/>
       <c r="T14" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="U14"/>
       <c r="V14"/>
@@ -4494,7 +4563,7 @@
         <v>65</v>
       </c>
       <c r="E15" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F15" t="s">
         <v>66</v>
@@ -4510,20 +4579,20 @@
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N15" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="R15"/>
       <c r="S15"/>
       <c r="T15" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="U15"/>
       <c r="V15"/>
@@ -4538,7 +4607,7 @@
         <v>67</v>
       </c>
       <c r="E16" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="F16" t="s">
         <v>68</v>
@@ -4572,7 +4641,7 @@
         <v>70</v>
       </c>
       <c r="E17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="F17" t="s">
         <v>71</v>
@@ -4608,7 +4677,7 @@
         <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F18" t="s">
         <v>77</v>
@@ -4621,25 +4690,25 @@
       </c>
       <c r="I18"/>
       <c r="J18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="N18" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="O18"/>
       <c r="P18"/>
       <c r="Q18" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="R18"/>
       <c r="S18"/>
       <c r="T18" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="U18"/>
       <c r="V18"/>
@@ -4665,25 +4734,25 @@
       </c>
       <c r="I19"/>
       <c r="J19" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="K19"/>
       <c r="L19"/>
       <c r="M19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="N19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="O19"/>
       <c r="P19"/>
       <c r="Q19" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="R19"/>
       <c r="S19"/>
       <c r="T19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="U19"/>
       <c r="V19"/>
@@ -4698,7 +4767,7 @@
         <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F20" t="s">
         <v>84</v>
@@ -4711,25 +4780,25 @@
       </c>
       <c r="I20"/>
       <c r="J20" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K20"/>
       <c r="L20"/>
       <c r="M20" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="N20" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="O20"/>
       <c r="P20"/>
       <c r="Q20" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="R20"/>
       <c r="S20"/>
       <c r="T20" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="U20"/>
       <c r="V20"/>
@@ -4744,7 +4813,7 @@
         <v>87</v>
       </c>
       <c r="E21" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="F21" t="s">
         <v>88</v>
@@ -4757,7 +4826,7 @@
       </c>
       <c r="I21"/>
       <c r="J21" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="K21"/>
       <c r="L21"/>
@@ -4766,12 +4835,12 @@
       <c r="O21"/>
       <c r="P21"/>
       <c r="Q21" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="R21"/>
       <c r="S21"/>
       <c r="T21" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="U21"/>
       <c r="V21"/>
@@ -5054,7 +5123,7 @@
         <v>126</v>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D30" t="s">
         <v>127</v>
@@ -5069,39 +5138,27 @@
       <c r="H30" t="s">
         <v>64</v>
       </c>
-      <c r="I30" t="s">
-        <v>130</v>
-      </c>
+      <c r="I30"/>
       <c r="J30" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K30" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L30"/>
       <c r="M30" t="s">
-        <v>306</v>
-      </c>
-      <c r="N30" t="s">
-        <v>307</v>
-      </c>
+        <v>304</v>
+      </c>
+      <c r="N30"/>
       <c r="O30" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="P30"/>
-      <c r="Q30" t="s">
-        <v>309</v>
-      </c>
-      <c r="R30" t="s">
-        <v>310</v>
-      </c>
+      <c r="Q30"/>
+      <c r="R30"/>
       <c r="S30"/>
-      <c r="T30" t="s">
-        <v>311</v>
-      </c>
-      <c r="U30" t="s">
-        <v>312</v>
-      </c>
+      <c r="T30"/>
+      <c r="U30"/>
       <c r="V30"/>
     </row>
     <row r="31">
@@ -5109,44 +5166,62 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" t="n">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>130</v>
+      </c>
+      <c r="E31" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" t="s">
         <v>132</v>
       </c>
-      <c r="C31" t="n">
-        <v>10</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="G31" t="s">
         <v>133</v>
       </c>
-      <c r="E31" t="s">
-        <v>134</v>
-      </c>
-      <c r="F31" t="s">
-        <v>135</v>
-      </c>
-      <c r="G31"/>
       <c r="H31" t="s">
         <v>64</v>
       </c>
-      <c r="I31"/>
+      <c r="I31" t="s">
+        <v>134</v>
+      </c>
       <c r="J31"/>
       <c r="K31"/>
       <c r="L31"/>
       <c r="M31" t="s">
+        <v>306</v>
+      </c>
+      <c r="N31" t="s">
+        <v>130</v>
+      </c>
+      <c r="O31" t="s">
+        <v>307</v>
+      </c>
+      <c r="P31" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>309</v>
+      </c>
+      <c r="R31" t="s">
+        <v>310</v>
+      </c>
+      <c r="S31" t="s">
+        <v>311</v>
+      </c>
+      <c r="T31" t="s">
+        <v>312</v>
+      </c>
+      <c r="U31" t="s">
         <v>313</v>
       </c>
-      <c r="N31"/>
-      <c r="O31"/>
-      <c r="P31"/>
-      <c r="Q31" t="s">
+      <c r="V31" t="s">
         <v>314</v>
       </c>
-      <c r="R31"/>
-      <c r="S31"/>
-      <c r="T31" t="s">
-        <v>133</v>
-      </c>
-      <c r="U31"/>
-      <c r="V31"/>
     </row>
     <row r="32">
       <c r="A32" t="s">
@@ -5156,7 +5231,7 @@
         <v>126</v>
       </c>
       <c r="C32" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
         <v>136</v>
@@ -5167,94 +5242,88 @@
       <c r="F32" t="s">
         <v>138</v>
       </c>
-      <c r="G32" t="s">
-        <v>139</v>
-      </c>
+      <c r="G32"/>
       <c r="H32" t="s">
         <v>64</v>
       </c>
-      <c r="I32" t="s">
-        <v>140</v>
-      </c>
-      <c r="J32" t="s">
-        <v>315</v>
-      </c>
-      <c r="K32" t="s">
-        <v>316</v>
-      </c>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
       <c r="L32"/>
       <c r="M32" t="s">
+        <v>315</v>
+      </c>
+      <c r="N32"/>
+      <c r="O32" t="s">
+        <v>316</v>
+      </c>
+      <c r="P32" t="s">
         <v>317</v>
       </c>
-      <c r="N32" t="s">
+      <c r="Q32" t="s">
         <v>318</v>
       </c>
-      <c r="O32" t="s">
+      <c r="R32" t="s">
+        <v>310</v>
+      </c>
+      <c r="S32" t="s">
         <v>319</v>
       </c>
-      <c r="P32"/>
-      <c r="Q32" t="s">
-        <v>320</v>
-      </c>
-      <c r="R32" t="s">
-        <v>316</v>
-      </c>
-      <c r="S32"/>
       <c r="T32" t="s">
         <v>136</v>
       </c>
       <c r="U32" t="s">
-        <v>321</v>
-      </c>
-      <c r="V32"/>
+        <v>320</v>
+      </c>
+      <c r="V32" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C33" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D33" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E33" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="F33" t="s">
-        <v>144</v>
-      </c>
-      <c r="G33" t="s">
-        <v>139</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="G33"/>
       <c r="H33" t="s">
         <v>64</v>
       </c>
       <c r="I33" t="s">
-        <v>140</v>
-      </c>
-      <c r="J33"/>
+        <v>19</v>
+      </c>
+      <c r="J33" t="s">
+        <v>139</v>
+      </c>
       <c r="K33"/>
       <c r="L33"/>
       <c r="M33" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N33" t="s">
-        <v>323</v>
+        <v>139</v>
       </c>
       <c r="O33"/>
       <c r="P33"/>
       <c r="Q33" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="R33"/>
       <c r="S33"/>
-      <c r="T33" t="s">
-        <v>325</v>
-      </c>
+      <c r="T33"/>
       <c r="U33"/>
       <c r="V33"/>
     </row>
@@ -5263,93 +5332,115 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C34" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D34" t="s">
+        <v>144</v>
+      </c>
+      <c r="E34" t="s">
         <v>145</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>146</v>
-      </c>
-      <c r="F34" t="s">
-        <v>147</v>
       </c>
       <c r="G34"/>
       <c r="H34" t="s">
         <v>64</v>
       </c>
       <c r="I34" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="J34" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="K34" t="s">
-        <v>327</v>
-      </c>
-      <c r="L34"/>
-      <c r="M34" t="s">
-        <v>328</v>
-      </c>
-      <c r="N34" t="s">
-        <v>329</v>
-      </c>
+        <v>324</v>
+      </c>
+      <c r="L34" t="s">
+        <v>325</v>
+      </c>
+      <c r="M34"/>
+      <c r="N34"/>
       <c r="O34"/>
       <c r="P34"/>
       <c r="Q34" t="s">
+        <v>326</v>
+      </c>
+      <c r="R34" t="s">
+        <v>327</v>
+      </c>
+      <c r="S34" t="s">
+        <v>328</v>
+      </c>
+      <c r="T34" t="s">
+        <v>329</v>
+      </c>
+      <c r="U34" t="s">
         <v>330</v>
       </c>
-      <c r="R34"/>
-      <c r="S34"/>
-      <c r="T34" t="s">
-        <v>331</v>
-      </c>
-      <c r="U34" t="s">
-        <v>321</v>
-      </c>
-      <c r="V34"/>
+      <c r="V34" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C35" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D35" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" t="s">
         <v>149</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>150</v>
-      </c>
-      <c r="F35" t="s">
-        <v>151</v>
       </c>
       <c r="G35"/>
       <c r="H35" t="s">
         <v>64</v>
       </c>
-      <c r="I35"/>
+      <c r="I35" t="s">
+        <v>147</v>
+      </c>
       <c r="J35" t="s">
+        <v>331</v>
+      </c>
+      <c r="K35" t="s">
         <v>332</v>
       </c>
-      <c r="K35"/>
-      <c r="L35"/>
+      <c r="L35" t="s">
+        <v>314</v>
+      </c>
       <c r="M35" t="s">
         <v>333</v>
       </c>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
+      <c r="N35" t="s">
+        <v>334</v>
+      </c>
+      <c r="O35" t="s">
+        <v>335</v>
+      </c>
+      <c r="P35" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>336</v>
+      </c>
+      <c r="R35" t="s">
+        <v>337</v>
+      </c>
+      <c r="S35" t="s">
+        <v>338</v>
+      </c>
       <c r="T35"/>
       <c r="U35"/>
       <c r="V35"/>
@@ -5359,10 +5450,10 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C36" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
         <v>152</v>
@@ -5378,37 +5469,57 @@
         <v>64</v>
       </c>
       <c r="I36" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="J36" t="s">
-        <v>334</v>
-      </c>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
+        <v>339</v>
+      </c>
+      <c r="K36" t="s">
+        <v>340</v>
+      </c>
+      <c r="L36" t="s">
+        <v>341</v>
+      </c>
+      <c r="M36" t="s">
+        <v>342</v>
+      </c>
+      <c r="N36" t="s">
+        <v>343</v>
+      </c>
+      <c r="O36" t="s">
+        <v>344</v>
+      </c>
+      <c r="P36" t="s">
+        <v>341</v>
+      </c>
       <c r="Q36" t="s">
-        <v>335</v>
-      </c>
-      <c r="R36"/>
-      <c r="S36"/>
+        <v>345</v>
+      </c>
+      <c r="R36" t="s">
+        <v>346</v>
+      </c>
+      <c r="S36" t="s">
+        <v>341</v>
+      </c>
       <c r="T36" t="s">
-        <v>336</v>
-      </c>
-      <c r="U36"/>
-      <c r="V36"/>
+        <v>347</v>
+      </c>
+      <c r="U36" t="s">
+        <v>348</v>
+      </c>
+      <c r="V36" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C37" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D37" t="s">
         <v>155</v>
@@ -5424,24 +5535,16 @@
         <v>64</v>
       </c>
       <c r="I37" t="s">
-        <v>19</v>
-      </c>
-      <c r="J37" t="s">
-        <v>155</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="J37"/>
       <c r="K37"/>
       <c r="L37"/>
-      <c r="M37" t="s">
-        <v>337</v>
-      </c>
-      <c r="N37" t="s">
-        <v>155</v>
-      </c>
+      <c r="M37"/>
+      <c r="N37"/>
       <c r="O37"/>
       <c r="P37"/>
-      <c r="Q37" t="s">
-        <v>338</v>
-      </c>
+      <c r="Q37"/>
       <c r="R37"/>
       <c r="S37"/>
       <c r="T37"/>
@@ -5453,10 +5556,10 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C38" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
         <v>159</v>
@@ -5467,89 +5570,103 @@
       <c r="F38" t="s">
         <v>161</v>
       </c>
-      <c r="G38"/>
+      <c r="G38" t="s">
+        <v>133</v>
+      </c>
       <c r="H38" t="s">
         <v>64</v>
       </c>
       <c r="I38" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="J38" t="s">
-        <v>339</v>
-      </c>
-      <c r="K38"/>
+        <v>349</v>
+      </c>
+      <c r="K38" t="s">
+        <v>350</v>
+      </c>
       <c r="L38"/>
       <c r="M38" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="N38" t="s">
-        <v>341</v>
-      </c>
-      <c r="O38"/>
-      <c r="P38"/>
+        <v>352</v>
+      </c>
+      <c r="O38" t="s">
+        <v>353</v>
+      </c>
+      <c r="P38" t="s">
+        <v>354</v>
+      </c>
       <c r="Q38" t="s">
-        <v>342</v>
-      </c>
-      <c r="R38"/>
-      <c r="S38"/>
-      <c r="T38"/>
-      <c r="U38"/>
-      <c r="V38"/>
+        <v>355</v>
+      </c>
+      <c r="R38" t="s">
+        <v>350</v>
+      </c>
+      <c r="S38" t="s">
+        <v>354</v>
+      </c>
+      <c r="T38" t="s">
+        <v>159</v>
+      </c>
+      <c r="U38" t="s">
+        <v>320</v>
+      </c>
+      <c r="V38" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
         <v>7</v>
       </c>
       <c r="B39" t="s">
+        <v>143</v>
+      </c>
+      <c r="C39" t="n">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
         <v>162</v>
       </c>
-      <c r="C39" t="n">
-        <v>14</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>163</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>164</v>
-      </c>
-      <c r="F39" t="s">
-        <v>165</v>
       </c>
       <c r="G39"/>
       <c r="H39" t="s">
         <v>64</v>
       </c>
       <c r="I39" t="s">
-        <v>130</v>
-      </c>
-      <c r="J39" t="s">
-        <v>343</v>
-      </c>
-      <c r="K39" t="s">
-        <v>344</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="J39"/>
+      <c r="K39"/>
       <c r="L39"/>
       <c r="M39" t="s">
-        <v>345</v>
-      </c>
-      <c r="N39" t="s">
-        <v>346</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="N39"/>
       <c r="O39" t="s">
-        <v>347</v>
-      </c>
-      <c r="P39"/>
-      <c r="Q39"/>
+        <v>357</v>
+      </c>
+      <c r="P39" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>358</v>
+      </c>
       <c r="R39" t="s">
-        <v>348</v>
-      </c>
-      <c r="S39"/>
-      <c r="T39" t="s">
-        <v>349</v>
-      </c>
-      <c r="U39" t="s">
-        <v>350</v>
-      </c>
+        <v>359</v>
+      </c>
+      <c r="S39" t="s">
+        <v>360</v>
+      </c>
+      <c r="T39"/>
+      <c r="U39"/>
       <c r="V39"/>
     </row>
     <row r="40">
@@ -5557,47 +5674,57 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C40" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D40" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" t="s">
         <v>166</v>
       </c>
-      <c r="E40" t="s">
+      <c r="F40" t="s">
         <v>167</v>
-      </c>
-      <c r="F40" t="s">
-        <v>168</v>
       </c>
       <c r="G40"/>
       <c r="H40" t="s">
         <v>64</v>
       </c>
       <c r="I40" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="J40" t="s">
-        <v>351</v>
-      </c>
-      <c r="K40"/>
+        <v>361</v>
+      </c>
+      <c r="K40" t="s">
+        <v>316</v>
+      </c>
       <c r="L40"/>
       <c r="M40" t="s">
-        <v>352</v>
+        <v>362</v>
       </c>
       <c r="N40" t="s">
-        <v>353</v>
-      </c>
-      <c r="O40"/>
+        <v>363</v>
+      </c>
+      <c r="O40" t="s">
+        <v>364</v>
+      </c>
       <c r="P40"/>
       <c r="Q40" t="s">
-        <v>354</v>
-      </c>
-      <c r="R40"/>
+        <v>365</v>
+      </c>
+      <c r="R40" t="s">
+        <v>310</v>
+      </c>
       <c r="S40"/>
-      <c r="T40"/>
-      <c r="U40"/>
+      <c r="T40" t="s">
+        <v>366</v>
+      </c>
+      <c r="U40" t="s">
+        <v>320</v>
+      </c>
       <c r="V40"/>
     </row>
     <row r="41">
@@ -5605,10 +5732,10 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="C41" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D41" t="s">
         <v>169</v>
@@ -5619,50 +5746,46 @@
       <c r="F41" t="s">
         <v>171</v>
       </c>
-      <c r="G41" t="s">
-        <v>139</v>
-      </c>
+      <c r="G41"/>
       <c r="H41" t="s">
         <v>64</v>
       </c>
       <c r="I41" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="J41" t="s">
-        <v>355</v>
+        <v>367</v>
       </c>
       <c r="K41" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="L41" t="s">
-        <v>356</v>
+        <v>368</v>
       </c>
       <c r="M41" t="s">
-        <v>357</v>
+        <v>369</v>
       </c>
       <c r="N41" t="s">
-        <v>358</v>
+        <v>370</v>
       </c>
       <c r="O41" t="s">
-        <v>347</v>
-      </c>
-      <c r="P41"/>
-      <c r="Q41"/>
+        <v>307</v>
+      </c>
+      <c r="P41" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>371</v>
+      </c>
       <c r="R41" t="s">
-        <v>348</v>
-      </c>
-      <c r="S41" t="n">
-        <v>88</v>
-      </c>
-      <c r="T41" t="s">
-        <v>359</v>
-      </c>
-      <c r="U41" t="s">
-        <v>350</v>
-      </c>
-      <c r="V41" t="s">
-        <v>360</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="S41" t="s">
+        <v>368</v>
+      </c>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
     </row>
     <row r="42">
       <c r="A42" t="s">
@@ -5672,7 +5795,7 @@
         <v>172</v>
       </c>
       <c r="C42" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D42" t="s">
         <v>173</v>
@@ -5684,33 +5807,47 @@
         <v>175</v>
       </c>
       <c r="G42" t="s">
-        <v>176</v>
+        <v>133</v>
       </c>
       <c r="H42" t="s">
         <v>64</v>
       </c>
       <c r="I42" t="s">
-        <v>177</v>
-      </c>
-      <c r="J42"/>
-      <c r="K42"/>
-      <c r="L42"/>
+        <v>134</v>
+      </c>
+      <c r="J42" t="s">
+        <v>372</v>
+      </c>
+      <c r="K42" t="s">
+        <v>373</v>
+      </c>
+      <c r="L42" t="s">
+        <v>374</v>
+      </c>
       <c r="M42" t="s">
-        <v>361</v>
-      </c>
-      <c r="N42"/>
-      <c r="O42"/>
-      <c r="P42"/>
+        <v>375</v>
+      </c>
+      <c r="N42" t="s">
+        <v>376</v>
+      </c>
+      <c r="O42" t="s">
+        <v>377</v>
+      </c>
+      <c r="P42" t="s">
+        <v>378</v>
+      </c>
       <c r="Q42"/>
       <c r="R42"/>
       <c r="S42"/>
       <c r="T42" t="s">
-        <v>173</v>
+        <v>379</v>
       </c>
       <c r="U42" t="s">
-        <v>362</v>
-      </c>
-      <c r="V42"/>
+        <v>380</v>
+      </c>
+      <c r="V42" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
@@ -5720,103 +5857,105 @@
         <v>172</v>
       </c>
       <c r="C43" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D43" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E43" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F43" t="s">
-        <v>181</v>
-      </c>
-      <c r="G43" t="s">
-        <v>139</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="G43"/>
       <c r="H43" t="s">
         <v>64</v>
       </c>
       <c r="I43" t="s">
-        <v>140</v>
-      </c>
-      <c r="J43"/>
-      <c r="K43"/>
-      <c r="L43"/>
+        <v>147</v>
+      </c>
+      <c r="J43" t="s">
+        <v>382</v>
+      </c>
+      <c r="K43" t="s">
+        <v>373</v>
+      </c>
+      <c r="L43" t="s">
+        <v>383</v>
+      </c>
       <c r="M43" t="s">
-        <v>363</v>
-      </c>
-      <c r="N43"/>
-      <c r="O43"/>
-      <c r="P43"/>
+        <v>384</v>
+      </c>
+      <c r="N43" t="s">
+        <v>385</v>
+      </c>
+      <c r="O43" t="s">
+        <v>377</v>
+      </c>
+      <c r="P43" t="s">
+        <v>383</v>
+      </c>
       <c r="Q43"/>
       <c r="R43"/>
       <c r="S43"/>
       <c r="T43" t="s">
-        <v>364</v>
+        <v>386</v>
       </c>
       <c r="U43" t="s">
-        <v>365</v>
-      </c>
-      <c r="V43"/>
+        <v>380</v>
+      </c>
+      <c r="V43" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
         <v>7</v>
       </c>
       <c r="B44" t="s">
+        <v>179</v>
+      </c>
+      <c r="C44" t="n">
+        <v>16</v>
+      </c>
+      <c r="D44" t="s">
+        <v>180</v>
+      </c>
+      <c r="E44" t="s">
+        <v>181</v>
+      </c>
+      <c r="F44" t="s">
         <v>182</v>
       </c>
-      <c r="C44" t="n">
-        <v>18</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="G44" t="s">
         <v>183</v>
-      </c>
-      <c r="E44" t="s">
-        <v>184</v>
-      </c>
-      <c r="F44" t="s">
-        <v>185</v>
-      </c>
-      <c r="G44" t="s">
-        <v>186</v>
       </c>
       <c r="H44" t="s">
         <v>64</v>
       </c>
       <c r="I44" t="s">
-        <v>187</v>
-      </c>
-      <c r="J44" t="s">
-        <v>183</v>
-      </c>
-      <c r="K44" t="s">
-        <v>366</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="J44"/>
+      <c r="K44"/>
       <c r="L44"/>
       <c r="M44" t="s">
-        <v>183</v>
-      </c>
-      <c r="N44" t="s">
-        <v>183</v>
-      </c>
+        <v>387</v>
+      </c>
+      <c r="N44"/>
       <c r="O44" t="s">
-        <v>367</v>
+        <v>388</v>
       </c>
       <c r="P44"/>
-      <c r="Q44" t="s">
-        <v>368</v>
-      </c>
-      <c r="R44" t="s">
-        <v>369</v>
-      </c>
+      <c r="Q44"/>
+      <c r="R44"/>
       <c r="S44"/>
       <c r="T44" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="U44" t="s">
-        <v>366</v>
+        <v>388</v>
       </c>
       <c r="V44"/>
     </row>
@@ -5825,269 +5964,287 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C45" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E45" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F45" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="G45" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H45" t="s">
         <v>64</v>
       </c>
       <c r="I45" t="s">
-        <v>140</v>
-      </c>
-      <c r="J45" t="s">
-        <v>370</v>
-      </c>
-      <c r="K45" t="s">
-        <v>366</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="J45"/>
+      <c r="K45"/>
       <c r="L45"/>
       <c r="M45" t="s">
-        <v>371</v>
-      </c>
-      <c r="N45" t="s">
-        <v>372</v>
-      </c>
+        <v>389</v>
+      </c>
+      <c r="N45"/>
       <c r="O45" t="s">
-        <v>373</v>
-      </c>
-      <c r="P45"/>
-      <c r="Q45" t="s">
-        <v>374</v>
-      </c>
-      <c r="R45" t="s">
-        <v>369</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="P45" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q45"/>
+      <c r="R45"/>
       <c r="S45"/>
-      <c r="T45"/>
+      <c r="T45" t="s">
+        <v>392</v>
+      </c>
       <c r="U45" t="s">
-        <v>366</v>
-      </c>
-      <c r="V45"/>
+        <v>390</v>
+      </c>
+      <c r="V45" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
         <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C46" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D46" t="s">
+        <v>190</v>
+      </c>
+      <c r="E46" t="s">
+        <v>191</v>
+      </c>
+      <c r="F46" t="s">
         <v>192</v>
       </c>
-      <c r="E46" t="s">
+      <c r="G46" t="s">
         <v>193</v>
-      </c>
-      <c r="F46" t="s">
-        <v>194</v>
-      </c>
-      <c r="G46" t="s">
-        <v>139</v>
       </c>
       <c r="H46" t="s">
         <v>64</v>
       </c>
       <c r="I46" t="s">
-        <v>140</v>
-      </c>
-      <c r="J46" t="s">
-        <v>375</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="J46"/>
       <c r="K46" t="s">
-        <v>366</v>
+        <v>393</v>
       </c>
       <c r="L46"/>
       <c r="M46" t="s">
-        <v>376</v>
-      </c>
-      <c r="N46" t="s">
-        <v>377</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="N46"/>
       <c r="O46" t="s">
-        <v>367</v>
-      </c>
-      <c r="P46"/>
+        <v>394</v>
+      </c>
+      <c r="P46" t="s">
+        <v>395</v>
+      </c>
       <c r="Q46"/>
-      <c r="R46" t="s">
-        <v>369</v>
-      </c>
+      <c r="R46"/>
       <c r="S46"/>
-      <c r="T46"/>
+      <c r="T46" t="s">
+        <v>190</v>
+      </c>
       <c r="U46" t="s">
-        <v>366</v>
-      </c>
-      <c r="V46"/>
+        <v>393</v>
+      </c>
+      <c r="V46" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
         <v>7</v>
       </c>
       <c r="B47" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C47" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D47" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E47" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F47" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G47" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="H47" t="s">
         <v>64</v>
       </c>
       <c r="I47" t="s">
-        <v>187</v>
-      </c>
-      <c r="J47"/>
+        <v>194</v>
+      </c>
+      <c r="J47" t="s">
+        <v>196</v>
+      </c>
       <c r="K47" t="s">
-        <v>366</v>
-      </c>
-      <c r="L47"/>
+        <v>393</v>
+      </c>
+      <c r="L47" t="s">
+        <v>395</v>
+      </c>
       <c r="M47" t="s">
-        <v>195</v>
-      </c>
-      <c r="N47"/>
+        <v>196</v>
+      </c>
+      <c r="N47" t="s">
+        <v>196</v>
+      </c>
       <c r="O47" t="s">
-        <v>378</v>
-      </c>
-      <c r="P47"/>
-      <c r="Q47"/>
+        <v>396</v>
+      </c>
+      <c r="P47" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>397</v>
+      </c>
       <c r="R47" t="s">
-        <v>369</v>
-      </c>
-      <c r="S47"/>
+        <v>398</v>
+      </c>
+      <c r="S47" t="s">
+        <v>395</v>
+      </c>
       <c r="T47" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="U47" t="s">
-        <v>366</v>
-      </c>
-      <c r="V47"/>
+        <v>393</v>
+      </c>
+      <c r="V47" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
         <v>7</v>
       </c>
       <c r="B48" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C48" t="n">
         <v>22</v>
       </c>
       <c r="D48" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E48" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F48" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="G48" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="H48" t="s">
         <v>64</v>
       </c>
       <c r="I48" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="J48"/>
       <c r="K48" t="s">
-        <v>366</v>
+        <v>393</v>
       </c>
       <c r="L48"/>
       <c r="M48" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="N48"/>
       <c r="O48" t="s">
-        <v>378</v>
-      </c>
-      <c r="P48"/>
+        <v>394</v>
+      </c>
+      <c r="P48" t="s">
+        <v>395</v>
+      </c>
       <c r="Q48"/>
       <c r="R48" t="s">
-        <v>369</v>
+        <v>398</v>
       </c>
       <c r="S48"/>
       <c r="T48" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="U48" t="s">
-        <v>366</v>
-      </c>
-      <c r="V48"/>
+        <v>393</v>
+      </c>
+      <c r="V48" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
         <v>7</v>
       </c>
       <c r="B49" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C49" t="n">
         <v>23</v>
       </c>
       <c r="D49" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E49" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F49" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G49" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H49" t="s">
         <v>64</v>
       </c>
       <c r="I49" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="J49" t="s">
-        <v>379</v>
+        <v>399</v>
       </c>
       <c r="K49" t="s">
-        <v>366</v>
-      </c>
-      <c r="L49"/>
+        <v>393</v>
+      </c>
+      <c r="L49" t="s">
+        <v>314</v>
+      </c>
       <c r="M49"/>
       <c r="N49"/>
-      <c r="O49" t="s">
-        <v>378</v>
-      </c>
+      <c r="O49"/>
       <c r="P49"/>
       <c r="Q49" t="s">
-        <v>380</v>
-      </c>
-      <c r="R49"/>
-      <c r="S49"/>
+        <v>400</v>
+      </c>
+      <c r="R49" t="s">
+        <v>398</v>
+      </c>
+      <c r="S49" t="s">
+        <v>401</v>
+      </c>
       <c r="T49"/>
       <c r="U49"/>
       <c r="V49"/>
@@ -6097,53 +6254,61 @@
         <v>7</v>
       </c>
       <c r="B50" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C50" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D50" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="E50" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F50" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G50" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H50" t="s">
         <v>64</v>
       </c>
       <c r="I50" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="J50" t="s">
-        <v>381</v>
+        <v>402</v>
       </c>
       <c r="K50" t="s">
-        <v>382</v>
-      </c>
-      <c r="L50"/>
+        <v>393</v>
+      </c>
+      <c r="L50" t="s">
+        <v>403</v>
+      </c>
       <c r="M50" t="s">
-        <v>383</v>
-      </c>
-      <c r="N50"/>
+        <v>404</v>
+      </c>
+      <c r="N50" t="s">
+        <v>405</v>
+      </c>
       <c r="O50" t="s">
-        <v>373</v>
-      </c>
-      <c r="P50"/>
-      <c r="Q50"/>
-      <c r="R50"/>
-      <c r="S50"/>
-      <c r="T50" t="s">
-        <v>384</v>
-      </c>
-      <c r="U50" t="s">
-        <v>373</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="P50" t="s">
+        <v>403</v>
+      </c>
+      <c r="Q50" t="s">
+        <v>407</v>
+      </c>
+      <c r="R50" t="s">
+        <v>398</v>
+      </c>
+      <c r="S50" t="s">
+        <v>401</v>
+      </c>
+      <c r="T50"/>
+      <c r="U50"/>
       <c r="V50"/>
     </row>
     <row r="51">
@@ -6151,49 +6316,55 @@
         <v>7</v>
       </c>
       <c r="B51" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C51" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D51" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E51" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F51" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="G51" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="H51" t="s">
         <v>64</v>
       </c>
       <c r="I51" t="s">
-        <v>140</v>
-      </c>
-      <c r="J51"/>
-      <c r="K51"/>
-      <c r="L51"/>
+        <v>134</v>
+      </c>
+      <c r="J51" t="s">
+        <v>408</v>
+      </c>
+      <c r="K51" t="s">
+        <v>393</v>
+      </c>
+      <c r="L51" t="s">
+        <v>403</v>
+      </c>
       <c r="M51" t="s">
-        <v>385</v>
-      </c>
-      <c r="N51"/>
+        <v>409</v>
+      </c>
+      <c r="N51" t="s">
+        <v>410</v>
+      </c>
       <c r="O51" t="s">
-        <v>373</v>
-      </c>
-      <c r="P51"/>
+        <v>396</v>
+      </c>
+      <c r="P51" t="s">
+        <v>403</v>
+      </c>
       <c r="Q51"/>
       <c r="R51"/>
       <c r="S51"/>
-      <c r="T51" t="s">
-        <v>386</v>
-      </c>
-      <c r="U51" t="s">
-        <v>373</v>
-      </c>
+      <c r="T51"/>
+      <c r="U51"/>
       <c r="V51"/>
     </row>
     <row r="52">
@@ -6201,167 +6372,209 @@
         <v>7</v>
       </c>
       <c r="B52" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="C52" t="n">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D52" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E52" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F52" t="s">
-        <v>212</v>
-      </c>
-      <c r="G52"/>
+        <v>213</v>
+      </c>
+      <c r="G52" t="s">
+        <v>133</v>
+      </c>
       <c r="H52" t="s">
         <v>64</v>
       </c>
       <c r="I52" t="s">
-        <v>130</v>
-      </c>
-      <c r="J52"/>
-      <c r="K52"/>
-      <c r="L52"/>
+        <v>134</v>
+      </c>
+      <c r="J52" t="s">
+        <v>411</v>
+      </c>
+      <c r="K52" t="s">
+        <v>412</v>
+      </c>
+      <c r="L52" t="s">
+        <v>413</v>
+      </c>
       <c r="M52" t="s">
-        <v>387</v>
+        <v>414</v>
       </c>
       <c r="N52"/>
-      <c r="O52"/>
-      <c r="P52"/>
-      <c r="Q52" t="s">
-        <v>388</v>
-      </c>
+      <c r="O52" t="s">
+        <v>406</v>
+      </c>
+      <c r="P52" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q52"/>
       <c r="R52"/>
       <c r="S52"/>
-      <c r="T52"/>
-      <c r="U52"/>
-      <c r="V52"/>
+      <c r="T52" t="s">
+        <v>415</v>
+      </c>
+      <c r="U52" t="s">
+        <v>406</v>
+      </c>
+      <c r="V52" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="C53" t="n">
-        <v>9</v>
-      </c>
-      <c r="D53"/>
+        <v>25</v>
+      </c>
+      <c r="D53" t="s">
+        <v>214</v>
+      </c>
       <c r="E53" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="F53" t="s">
-        <v>214</v>
-      </c>
-      <c r="G53"/>
-      <c r="H53"/>
-      <c r="I53"/>
+        <v>216</v>
+      </c>
+      <c r="G53" t="s">
+        <v>133</v>
+      </c>
+      <c r="H53" t="s">
+        <v>64</v>
+      </c>
+      <c r="I53" t="s">
+        <v>134</v>
+      </c>
       <c r="J53"/>
       <c r="K53"/>
       <c r="L53"/>
-      <c r="M53"/>
+      <c r="M53" t="s">
+        <v>416</v>
+      </c>
       <c r="N53"/>
-      <c r="O53"/>
-      <c r="P53"/>
+      <c r="O53" t="s">
+        <v>406</v>
+      </c>
+      <c r="P53" t="s">
+        <v>413</v>
+      </c>
       <c r="Q53"/>
       <c r="R53"/>
       <c r="S53"/>
-      <c r="T53"/>
+      <c r="T53" t="s">
+        <v>417</v>
+      </c>
       <c r="U53" t="s">
-        <v>389</v>
-      </c>
-      <c r="V53"/>
+        <v>406</v>
+      </c>
+      <c r="V53" t="s">
+        <v>413</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
         <v>7</v>
       </c>
       <c r="B54" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C54" t="n">
         <v>60</v>
       </c>
       <c r="D54" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="E54" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="F54" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="G54"/>
       <c r="H54" t="s">
         <v>64</v>
       </c>
       <c r="I54" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="J54"/>
-      <c r="K54" t="s">
-        <v>390</v>
-      </c>
+      <c r="K54"/>
       <c r="L54"/>
       <c r="M54"/>
       <c r="N54"/>
       <c r="O54"/>
       <c r="P54"/>
       <c r="Q54" t="s">
-        <v>391</v>
-      </c>
-      <c r="R54"/>
-      <c r="S54"/>
+        <v>418</v>
+      </c>
+      <c r="R54" t="s">
+        <v>419</v>
+      </c>
+      <c r="S54" t="s">
+        <v>314</v>
+      </c>
       <c r="T54" t="s">
-        <v>392</v>
+        <v>420</v>
       </c>
       <c r="U54" t="s">
-        <v>393</v>
-      </c>
-      <c r="V54"/>
+        <v>421</v>
+      </c>
+      <c r="V54" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
         <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C55" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D55" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="E55" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F55" t="s">
-        <v>221</v>
-      </c>
-      <c r="G55"/>
+        <v>222</v>
+      </c>
+      <c r="G55" t="s">
+        <v>223</v>
+      </c>
       <c r="H55" t="s">
         <v>64</v>
       </c>
       <c r="I55" t="s">
-        <v>222</v>
+        <v>19</v>
       </c>
       <c r="J55"/>
       <c r="K55"/>
       <c r="L55"/>
       <c r="M55" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="N55"/>
-      <c r="O55"/>
-      <c r="P55"/>
-      <c r="Q55" t="s">
-        <v>394</v>
-      </c>
+      <c r="O55" t="s">
+        <v>422</v>
+      </c>
+      <c r="P55" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q55"/>
       <c r="R55"/>
       <c r="S55"/>
       <c r="T55"/>
@@ -6373,41 +6586,51 @@
         <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C56" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D56" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E56" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F56" t="s">
-        <v>225</v>
-      </c>
-      <c r="G56"/>
+        <v>227</v>
+      </c>
+      <c r="G56" t="s">
+        <v>228</v>
+      </c>
       <c r="H56" t="s">
         <v>64</v>
       </c>
       <c r="I56" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="J56"/>
       <c r="K56"/>
       <c r="L56"/>
       <c r="M56" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="N56"/>
-      <c r="O56"/>
-      <c r="P56"/>
+      <c r="O56" t="s">
+        <v>422</v>
+      </c>
+      <c r="P56" t="s">
+        <v>422</v>
+      </c>
       <c r="Q56" t="s">
-        <v>395</v>
-      </c>
-      <c r="R56"/>
-      <c r="S56"/>
+        <v>423</v>
+      </c>
+      <c r="R56" t="s">
+        <v>424</v>
+      </c>
+      <c r="S56" t="s">
+        <v>314</v>
+      </c>
       <c r="T56"/>
       <c r="U56"/>
       <c r="V56"/>
@@ -6417,43 +6640,49 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C57" t="n">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D57" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="E57" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="F57" t="s">
-        <v>228</v>
-      </c>
-      <c r="G57" t="s">
-        <v>229</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="G57"/>
       <c r="H57" t="s">
         <v>64</v>
       </c>
       <c r="I57" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="J57"/>
       <c r="K57"/>
       <c r="L57"/>
       <c r="M57" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="N57"/>
-      <c r="O57"/>
-      <c r="P57"/>
+      <c r="O57" t="s">
+        <v>422</v>
+      </c>
+      <c r="P57" t="s">
+        <v>314</v>
+      </c>
       <c r="Q57" t="s">
-        <v>396</v>
-      </c>
-      <c r="R57"/>
-      <c r="S57"/>
+        <v>425</v>
+      </c>
+      <c r="R57" t="s">
+        <v>426</v>
+      </c>
+      <c r="S57" t="s">
+        <v>314</v>
+      </c>
       <c r="T57"/>
       <c r="U57"/>
       <c r="V57"/>
@@ -6463,45 +6692,51 @@
         <v>7</v>
       </c>
       <c r="B58" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C58" t="n">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D58" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E58" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="F58" t="s">
-        <v>233</v>
-      </c>
-      <c r="G58" t="s">
-        <v>234</v>
-      </c>
+        <v>237</v>
+      </c>
+      <c r="G58"/>
       <c r="H58" t="s">
         <v>64</v>
       </c>
       <c r="I58" t="s">
-        <v>19</v>
+        <v>234</v>
       </c>
       <c r="J58"/>
       <c r="K58"/>
       <c r="L58"/>
       <c r="M58" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="N58"/>
-      <c r="O58"/>
-      <c r="P58"/>
-      <c r="Q58"/>
-      <c r="R58"/>
-      <c r="S58"/>
+      <c r="O58" t="s">
+        <v>422</v>
+      </c>
+      <c r="P58" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q58" t="s">
+        <v>427</v>
+      </c>
+      <c r="R58" t="s">
+        <v>426</v>
+      </c>
+      <c r="S58" t="s">
+        <v>314</v>
+      </c>
       <c r="T58"/>
-      <c r="U58" t="s">
-        <v>393</v>
-      </c>
+      <c r="U58"/>
       <c r="V58"/>
     </row>
     <row r="59">
@@ -6509,86 +6744,50 @@
         <v>7</v>
       </c>
       <c r="B59" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C59" t="n">
         <v>65</v>
       </c>
       <c r="D59" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E59" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="F59" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="G59"/>
       <c r="H59" t="s">
         <v>64</v>
       </c>
       <c r="I59" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="J59"/>
       <c r="K59"/>
       <c r="L59"/>
       <c r="M59" t="s">
-        <v>397</v>
+        <v>428</v>
       </c>
       <c r="N59"/>
-      <c r="O59"/>
+      <c r="O59" t="s">
+        <v>429</v>
+      </c>
       <c r="P59"/>
       <c r="Q59" t="s">
-        <v>398</v>
-      </c>
-      <c r="R59"/>
-      <c r="S59"/>
+        <v>430</v>
+      </c>
+      <c r="R59" t="s">
+        <v>431</v>
+      </c>
+      <c r="S59" t="s">
+        <v>314</v>
+      </c>
       <c r="T59"/>
       <c r="U59"/>
       <c r="V59"/>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
-        <v>7</v>
-      </c>
-      <c r="B60" t="s">
-        <v>126</v>
-      </c>
-      <c r="C60" t="n">
-        <v>2</v>
-      </c>
-      <c r="D60" t="s">
-        <v>239</v>
-      </c>
-      <c r="E60" t="s">
-        <v>240</v>
-      </c>
-      <c r="F60" t="s">
-        <v>241</v>
-      </c>
-      <c r="G60"/>
-      <c r="H60" t="s">
-        <v>64</v>
-      </c>
-      <c r="I60" t="s">
-        <v>242</v>
-      </c>
-      <c r="J60"/>
-      <c r="K60" t="s">
-        <v>399</v>
-      </c>
-      <c r="L60"/>
-      <c r="M60"/>
-      <c r="N60"/>
-      <c r="O60"/>
-      <c r="P60"/>
-      <c r="Q60"/>
-      <c r="R60"/>
-      <c r="S60"/>
-      <c r="T60"/>
-      <c r="U60"/>
-      <c r="V60"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>